<commit_message>
Cập nhật toàn bộ dự án, tách máy chủ làm hai để đảm bảo bảo mật (ExamServer, ManagementServer), dựng code kết nối cho StudentApp
</commit_message>
<xml_diff>
--- a/PolyTest_ExamPaperTemplate.xlsx
+++ b/PolyTest_ExamPaperTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F776CB-386B-4E16-B8E4-73185BD92369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62EC2CD-78AF-4001-9126-F3E5C62E93A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="13920" windowHeight="21789" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin" sheetId="2" r:id="rId1"/>
@@ -453,7 +453,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -547,30 +547,26 @@
     <xf numFmtId="7" fontId="20" fillId="3" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -626,6 +622,26 @@
           <color theme="4" tint="-0.749992370372631"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -953,26 +969,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color theme="3"/>
         <name val="Franklin Gothic Medium"/>
         <family val="2"/>
@@ -1125,13 +1121,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Mã câu" dataDxfId="13" totalsRowDxfId="0" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Câu hỏi" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Table Text"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="A" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Table Text"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="B" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Table Text"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="C" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="D" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Đáp án" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Mã câu" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Câu hỏi" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Table Text"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="A" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Table Text"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="B" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Table Text"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="C" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="D" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Đáp án" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1371,7 +1367,7 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1382,7 +1378,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="41"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -1393,37 +1389,35 @@
       <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="39"/>
     </row>
     <row r="6" spans="2:9" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1446,18 +1440,18 @@
       <c r="C12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="38"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H14" s="3"/>
@@ -1516,8 +1510,8 @@
   </sheetPr>
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1538,7 +1532,7 @@
       </c>
     </row>
     <row r="2" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="26" t="s">
@@ -1569,7 +1563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
@@ -1749,12 +1743,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2058,29 +2063,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F853990A-E8CE-40A1-B16C-FF31E7264638}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504056B5-BF2F-4DFA-A57F-D75DA6DEA9DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2107,13 +2105,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504056B5-BF2F-4DFA-A57F-D75DA6DEA9DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F853990A-E8CE-40A1-B16C-FF31E7264638}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>